<commit_message>
update: changed package json
</commit_message>
<xml_diff>
--- a/concepts/monsters.xlsx
+++ b/concepts/monsters.xlsx
@@ -135,12 +135,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -155,8 +161,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,7 +447,7 @@
   <dimension ref="C3:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,7 +496,7 @@
       </c>
     </row>
     <row r="7" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D7" t="s">
@@ -503,7 +510,7 @@
       </c>
     </row>
     <row r="8" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D8" t="s">
@@ -618,7 +625,7 @@
       </c>
     </row>
     <row r="16" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D16" t="s">
@@ -632,7 +639,7 @@
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D17" t="s">
@@ -640,7 +647,7 @@
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D18" t="s">

</xml_diff>